<commit_message>
Add stem summary to notes
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VAI-splitstem.xlsx
+++ b/inc/flattened/createYaml/VAI-splitstem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C1ACE-80C7-1B42-88A9-3E5BAFC6A2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D17724-2B7F-4043-974E-78E8116D5A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36660" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{E4BD15C6-4400-1343-AC8C-A1FC41388A9F}"/>
   </bookViews>
@@ -4530,8 +4530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F2A357-C052-5C45-9A70-6AB7A159287E}">
   <dimension ref="A1:K721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A690" zoomScale="116" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A712" zoomScale="116" workbookViewId="0">
+      <selection activeCell="H707" sqref="H707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>